<commit_message>
Ulzii added for the Rest.
</commit_message>
<xml_diff>
--- a/Team Spark.xlsx
+++ b/Team Spark.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulzii-erdene-bulgan/git/teamSpark/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -206,16 +219,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,12 +304,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -326,12 +339,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -537,28 +550,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" zoomScalePageLayoutView="187" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>47</v>
       </c>
@@ -587,7 +600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -628,7 +641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -650,7 +663,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B27" si="0">B3+1</f>
@@ -670,7 +683,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
@@ -690,7 +703,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
@@ -710,7 +723,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
@@ -730,7 +743,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
@@ -752,7 +765,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
@@ -772,7 +785,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
@@ -792,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
@@ -812,7 +825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
@@ -832,7 +845,7 @@
       </c>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
@@ -852,7 +865,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <f t="shared" si="0"/>
@@ -874,7 +887,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <f t="shared" si="0"/>
@@ -896,7 +909,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <f t="shared" si="0"/>
@@ -916,7 +929,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
@@ -938,7 +951,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
@@ -960,7 +973,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
@@ -980,7 +993,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -1000,7 +1013,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -1020,7 +1033,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <f t="shared" si="0"/>
@@ -1040,7 +1053,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <f t="shared" si="0"/>
@@ -1062,7 +1075,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3">
         <f t="shared" si="0"/>
@@ -1084,7 +1097,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3">
         <f t="shared" si="0"/>
@@ -1106,7 +1119,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3">
         <f t="shared" si="0"/>
@@ -1128,7 +1141,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3">
         <f t="shared" si="0"/>
@@ -1150,7 +1163,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1179,7 +1192,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1191,7 +1204,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>